<commit_message>
QAKL: Review 232, 225
</commit_message>
<xml_diff>
--- a/QuizAndKeyList.xlsx
+++ b/QuizAndKeyList.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="255">
   <si>
     <t>No</t>
   </si>
@@ -635,9 +635,6 @@
     <t>Containers</t>
   </si>
   <si>
-    <t>(1) push(x), pop(), top(), empty()</t>
-  </si>
-  <si>
     <t>Power of Two</t>
   </si>
   <si>
@@ -648,9 +645,6 @@
   </si>
   <si>
     <t xml:space="preserve">Implement Queue Using Stacks </t>
-  </si>
-  <si>
-    <t>(1) push(x), pop(), peek(), empty()</t>
   </si>
   <si>
     <t>Lowest Common Ancestor Of A Binary Search Tree</t>
@@ -1077,6 +1071,81 @@
     <t>Reviewed</t>
     <phoneticPr fontId="7"/>
   </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PI:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> push(x), pop(), top(), empty()</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PI:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> push(x), pop(), peek(), empty()</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>用兩個</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Queue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>來做 pop取出時和top確認時 只要使用原本的API就好 分別是poll和peek 在push放入的時候需要做修改 每次push時都把Q1元素照順序取出放入Q2 才放入 把新元素加入空的Q1 再把Q2的元素們加回來 所以整串Q1裡面會一直是反向的存著元素們 因此取出時不需要另外處理</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>用兩個Stack來做 push放入時不用處理直接存到S1 在取出pop或確認top時 從上面取出 放入S2 (順序反過來) 再從S2上方取出或確認即可</t>
+    <phoneticPr fontId="7"/>
+  </si>
 </sst>
 </file>
 
@@ -1185,7 +1254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1254,11 +1323,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1631,8 +1708,8 @@
   <dimension ref="A1:AD1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1652,13 +1729,13 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
@@ -1708,7 +1785,7 @@
       <c r="AC1" s="6"/>
       <c r="AD1" s="6"/>
     </row>
-    <row r="2" spans="1:30" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" s="13" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1716,7 +1793,7 @@
         <v>43029</v>
       </c>
       <c r="C2" s="20">
-        <v>43029</v>
+        <v>43082</v>
       </c>
       <c r="D2" s="9">
         <v>232</v>
@@ -1725,24 +1802,32 @@
         <v>92</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>185</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="J2" s="9"/>
+        <v>246</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="K2" s="13">
+        <v>124</v>
+      </c>
+      <c r="L2" s="13">
+        <v>54</v>
+      </c>
       <c r="M2" s="17">
         <f t="shared" ref="M2:M33" si="0">IF(ISBLANK(K2),,((K2-L2*2)+1000)/9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>112.88888888888889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" s="13" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -1750,7 +1835,7 @@
         <v>43030</v>
       </c>
       <c r="C3" s="20">
-        <v>43030</v>
+        <v>43082</v>
       </c>
       <c r="D3" s="9">
         <v>225</v>
@@ -1765,15 +1850,23 @@
         <v>185</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="J3" s="9"/>
+        <v>246</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="K3" s="13">
+        <v>73</v>
+      </c>
+      <c r="L3" s="13">
+        <v>136</v>
+      </c>
       <c r="M3" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="13" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -1799,7 +1892,7 @@
         <v>25</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>156</v>
@@ -1835,7 +1928,7 @@
         <v>25</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>165</v>
@@ -1868,7 +1961,7 @@
         <v>126</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>34</v>
@@ -1904,7 +1997,7 @@
         <v>121</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>34</v>
@@ -1941,7 +2034,7 @@
         <v>41</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>119</v>
@@ -1977,7 +2070,7 @@
         <v>41</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>120</v>
@@ -2011,7 +2104,7 @@
         <v>41</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>119</v>
@@ -2045,7 +2138,7 @@
         <v>41</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>120</v>
@@ -2079,7 +2172,7 @@
         <v>41</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>145</v>
@@ -2109,19 +2202,19 @@
         <v>92</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>93</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M13" s="17">
         <f t="shared" si="0"/>
@@ -2145,19 +2238,19 @@
         <v>92</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>71</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M14" s="17">
         <f t="shared" si="0"/>
@@ -2217,7 +2310,7 @@
         <v>92</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>25</v>
@@ -2226,10 +2319,10 @@
         <v>26</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M16" s="17">
         <f t="shared" si="0"/>
@@ -2253,7 +2346,7 @@
         <v>29</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>25</v>
@@ -2262,10 +2355,10 @@
         <v>26</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M17" s="17">
         <f t="shared" si="0"/>
@@ -2361,7 +2454,7 @@
         <v>92</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>58</v>
@@ -2370,10 +2463,10 @@
         <v>59</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M20" s="17">
         <f t="shared" si="0"/>
@@ -2397,7 +2490,7 @@
         <v>92</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>58</v>
@@ -2406,10 +2499,10 @@
         <v>59</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M21" s="17">
         <f t="shared" si="0"/>
@@ -2433,7 +2526,7 @@
         <v>92</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>58</v>
@@ -2442,10 +2535,10 @@
         <v>59</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M22" s="17">
         <f t="shared" si="0"/>
@@ -2469,7 +2562,7 @@
         <v>92</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>58</v>
@@ -2478,10 +2571,10 @@
         <v>59</v>
       </c>
       <c r="I23" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="J23" s="9" t="s">
         <v>188</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>189</v>
       </c>
       <c r="M23" s="17">
         <f t="shared" si="0"/>
@@ -2505,7 +2598,7 @@
         <v>29</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>58</v>
@@ -2514,10 +2607,10 @@
         <v>59</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M24" s="17">
         <f t="shared" si="0"/>
@@ -2577,7 +2670,7 @@
         <v>92</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>58</v>
@@ -2586,10 +2679,10 @@
         <v>59</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M26" s="17">
         <f t="shared" si="0"/>
@@ -2649,7 +2742,7 @@
         <v>29</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>58</v>
@@ -2658,10 +2751,10 @@
         <v>59</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M28" s="17">
         <f t="shared" si="0"/>
@@ -2694,7 +2787,7 @@
         <v>26</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J29" s="9" t="s">
         <v>107</v>
@@ -3066,7 +3159,7 @@
         <v>92</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>96</v>
@@ -3075,10 +3168,10 @@
         <v>97</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K38" s="9">
         <v>96</v>
@@ -3108,19 +3201,19 @@
         <v>29</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>168</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K39" s="9">
         <v>56</v>
@@ -3318,7 +3411,7 @@
         <v>92</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>168</v>
@@ -3327,10 +3420,10 @@
         <v>178</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K44" s="9">
         <v>264</v>
@@ -3360,7 +3453,7 @@
         <v>92</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>25</v>
@@ -3369,10 +3462,10 @@
         <v>26</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K45" s="9">
         <v>434</v>
@@ -3476,19 +3569,19 @@
         <v>92</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>71</v>
       </c>
       <c r="H48" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="J48" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="I48" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="J48" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="K48" s="9">
         <v>257</v>
@@ -3738,7 +3831,7 @@
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="M66" s="18">
-        <f t="shared" ref="M66:M97" si="2">IF(ISBLANK(K66),,((K66-L66*2)+1000)/9)</f>
+        <f t="shared" ref="M66:M69" si="2">IF(ISBLANK(K66),,((K66-L66*2)+1000)/9)</f>
         <v>0</v>
       </c>
     </row>
@@ -11291,22 +11384,22 @@
   </sortState>
   <phoneticPr fontId="7"/>
   <conditionalFormatting sqref="M1:M1008">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1008">
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH(("Easy"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1008">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH(("Medium"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>43070</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17865,42 +17958,42 @@
   </sheetData>
   <phoneticPr fontId="7"/>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Algo">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Algo">
       <formula>NOT(ISERROR(SEARCH(("Algo"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Array">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Array">
       <formula>NOT(ISERROR(SEARCH(("Array"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Backtracking">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Backtracking">
       <formula>NOT(ISERROR(SEARCH(("Backtracking"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="DP">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="DP">
       <formula>NOT(ISERROR(SEARCH(("DP"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="LinkedList">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="LinkedList">
       <formula>NOT(ISERROR(SEARCH(("LinkedList"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Math">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Math">
       <formula>NOT(ISERROR(SEARCH(("Math"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="Tree">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Tree">
       <formula>NOT(ISERROR(SEARCH(("Tree"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="String">
+    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="String">
       <formula>NOT(ISERROR(SEARCH(("String"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
QAKL: Review 100, 101, 111, 112, 113, 226
</commit_message>
<xml_diff>
--- a/QuizAndKeyList.xlsx
+++ b/QuizAndKeyList.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g3094010\git\Note-Java\"/>
@@ -16,14 +16,14 @@
     <sheet name="SimpleList" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$1:$G$1007</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$1:$H$1008</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="281">
   <si>
     <t>No</t>
   </si>
@@ -516,9 +516,6 @@
   </si>
   <si>
     <t>tree</t>
-  </si>
-  <si>
-    <t>找出一棵樹的最大深度</t>
   </si>
   <si>
     <t>用DFS做。事前先開一個arr存兩個變數(目前深度，最大深度)
@@ -811,6 +808,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -827,6 +825,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 
 </t>
@@ -844,6 +843,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -860,6 +860,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -876,6 +877,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">array 
 </t>
@@ -893,6 +895,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -972,6 +975,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -988,6 +992,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">target </t>
     </r>
@@ -1022,6 +1027,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">target
 </t>
@@ -1039,6 +1045,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>index</t>
     </r>
@@ -1087,6 +1094,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> push(x), pop(), top(), empty()</t>
     </r>
@@ -1108,6 +1116,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> push(x), pop(), peek(), empty()</t>
     </r>
@@ -1146,15 +1155,1248 @@
     <t>用兩個Stack來做 push放入時不用處理直接存到S1 在取出pop或確認top時 從上面取出 放入S2 (順序反過來) 再從S2上方取出或確認即可</t>
     <phoneticPr fontId="7"/>
   </si>
+  <si>
+    <t xml:space="preserve">Done? </t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>Same Tree</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ree</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ree</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>asy</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>Easy</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>Path Sum</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>Path Sum 2</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy </t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>給一棵樹和一個</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target(int) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>判斷從</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>root</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>leaf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>的各條</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">path </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>有沒有任何一條的和加總會是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>回傳</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">boolean </t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>直覺的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">traverse </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>兩棵樹分別比較左右</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>一直到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">leaf </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>記得要注意</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>一開始先比較左右兩個節點</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>如果一樣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>做一個可以傳入兩個變數的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">helper </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>傳入左右子樹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>一直往下比較</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>可以用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Level-Traversal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>來做</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>一個</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>queue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>或兩個</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">queue) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>先碰到的葉子</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>該處的深度就是最小深度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Method2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>也可以直接用遞迴的方式往下找</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>直接看</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>可能比較快</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>簡單說分成兩種</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>case (1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>左樹或右樹有任何一邊為空</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>則該節點的最小高是左高</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>右高</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+1 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>其中左高或右高為</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0) (2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>兩邊都不為空</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>則最小高是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>min(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>左高</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>右高</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">)+1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>一路從下往上算</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>也是遞迴往下</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>做一個</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">helper(node, sum, target) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>當</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>node</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>兩邊都是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>的時候</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>檢查</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>是否等於</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>只要有一個</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>就一路跳出來</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>但</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>不能跳出來</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>要繼續檢查</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>一樣是遞回來做</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> helpe(n)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>內是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">templeft = helper(n.left) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>也就是翻轉左樹以下之後再把左樹接到右側</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> n.right=templeft </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>當然左右都要做</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>回傳本身</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">n </t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>給一棵樹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>回傳一棵樹的最大深度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>給兩棵樹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>回傳是否相同</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>給一棵樹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>回傳是否左右對稱</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>給一棵樹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>回傳一棵樹的最小深度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>延續</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">#112 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>給一棵樹和一個</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">target(int) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>不只是找出有沒有加總符合的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">path </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>要列出全部符合的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">path </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>回傳</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> List&lt;List&lt;Integer&gt;&gt;</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>給一棵樹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>回傳一棵樹與原樹左右對稱</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>#112</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">一樣的解法 差別在於要多傳兩個變數 一個是現在的List 一個是全部的ListList 然後作法就是往下的時候裝一個進去List 出來的時候拿掉一個最後面的元素 最後加入ListList的時候記得要用new的 不能直接加原本的List </t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1163,27 +2405,32 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF3C78D8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFA64D79"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1227,8 +2474,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1241,8 +2496,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1250,11 +2511,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1326,16 +2631,36 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1705,37 +3030,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="26.140625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="52.7109375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="58.7109375" customWidth="1"/>
+    <col min="9" max="9" width="52.7109375" style="37" customWidth="1"/>
+    <col min="10" max="10" width="58.7109375" style="27" customWidth="1"/>
     <col min="11" max="12" width="7.28515625" customWidth="1"/>
     <col min="13" max="13" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
@@ -1802,19 +3129,19 @@
         <v>92</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I2" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>252</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>253</v>
       </c>
       <c r="K2" s="13">
         <v>124</v>
@@ -1844,19 +3171,19 @@
         <v>92</v>
       </c>
       <c r="F3" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>185</v>
-      </c>
       <c r="H3" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K3" s="13">
         <v>73</v>
@@ -1892,13 +3219,13 @@
         <v>25</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I4" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="M4" s="17">
         <f t="shared" si="0"/>
@@ -1922,19 +3249,19 @@
         <v>29</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I5" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="M5" s="17">
         <f t="shared" si="0"/>
@@ -1961,7 +3288,7 @@
         <v>126</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>34</v>
@@ -1997,7 +3324,7 @@
         <v>121</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>34</v>
@@ -2034,7 +3361,7 @@
         <v>41</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>119</v>
@@ -2070,7 +3397,7 @@
         <v>41</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>120</v>
@@ -2104,7 +3431,7 @@
         <v>41</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>119</v>
@@ -2138,7 +3465,7 @@
         <v>41</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>120</v>
@@ -2172,7 +3499,7 @@
         <v>41</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>145</v>
@@ -2202,19 +3529,19 @@
         <v>92</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>93</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I13" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J13" s="9" t="s">
         <v>229</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>230</v>
       </c>
       <c r="M13" s="17">
         <f t="shared" si="0"/>
@@ -2238,19 +3565,19 @@
         <v>92</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>71</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I14" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="J14" s="9" t="s">
         <v>232</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>233</v>
       </c>
       <c r="M14" s="17">
         <f t="shared" si="0"/>
@@ -2274,7 +3601,7 @@
         <v>29</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>25</v>
@@ -2283,10 +3610,10 @@
         <v>26</v>
       </c>
       <c r="I15" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>183</v>
       </c>
       <c r="M15" s="17">
         <f t="shared" si="0"/>
@@ -2310,7 +3637,7 @@
         <v>92</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>25</v>
@@ -2319,10 +3646,10 @@
         <v>26</v>
       </c>
       <c r="I16" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>207</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>208</v>
       </c>
       <c r="M16" s="17">
         <f t="shared" si="0"/>
@@ -2346,7 +3673,7 @@
         <v>29</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>25</v>
@@ -2355,10 +3682,10 @@
         <v>26</v>
       </c>
       <c r="I17" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="M17" s="17">
         <f t="shared" si="0"/>
@@ -2382,7 +3709,7 @@
         <v>92</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>58</v>
@@ -2391,10 +3718,10 @@
         <v>59</v>
       </c>
       <c r="I18" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>176</v>
       </c>
       <c r="M18" s="17">
         <f t="shared" si="0"/>
@@ -2418,7 +3745,7 @@
         <v>92</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>58</v>
@@ -2427,10 +3754,10 @@
         <v>59</v>
       </c>
       <c r="I19" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="J19" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="M19" s="17">
         <f t="shared" si="0"/>
@@ -2454,7 +3781,7 @@
         <v>92</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>58</v>
@@ -2463,10 +3790,10 @@
         <v>59</v>
       </c>
       <c r="I20" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="J20" s="9" t="s">
         <v>198</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>199</v>
       </c>
       <c r="M20" s="17">
         <f t="shared" si="0"/>
@@ -2490,7 +3817,7 @@
         <v>92</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>58</v>
@@ -2499,10 +3826,10 @@
         <v>59</v>
       </c>
       <c r="I21" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="J21" s="9" t="s">
         <v>204</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>205</v>
       </c>
       <c r="M21" s="17">
         <f t="shared" si="0"/>
@@ -2526,7 +3853,7 @@
         <v>92</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>58</v>
@@ -2535,10 +3862,10 @@
         <v>59</v>
       </c>
       <c r="I22" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>210</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>211</v>
       </c>
       <c r="M22" s="17">
         <f t="shared" si="0"/>
@@ -2562,7 +3889,7 @@
         <v>92</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>58</v>
@@ -2571,10 +3898,10 @@
         <v>59</v>
       </c>
       <c r="I23" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="J23" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="M23" s="17">
         <f t="shared" si="0"/>
@@ -2598,7 +3925,7 @@
         <v>29</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>58</v>
@@ -2607,10 +3934,10 @@
         <v>59</v>
       </c>
       <c r="I24" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>201</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>202</v>
       </c>
       <c r="M24" s="17">
         <f t="shared" si="0"/>
@@ -2634,7 +3961,7 @@
         <v>92</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>58</v>
@@ -2643,10 +3970,10 @@
         <v>59</v>
       </c>
       <c r="I25" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="M25" s="17">
         <f t="shared" si="0"/>
@@ -2670,7 +3997,7 @@
         <v>92</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>58</v>
@@ -2679,10 +4006,10 @@
         <v>59</v>
       </c>
       <c r="I26" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>223</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>224</v>
       </c>
       <c r="M26" s="17">
         <f t="shared" si="0"/>
@@ -2706,7 +4033,7 @@
         <v>29</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>58</v>
@@ -2715,10 +4042,10 @@
         <v>59</v>
       </c>
       <c r="I27" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="J27" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="M27" s="17">
         <f t="shared" si="0"/>
@@ -2742,7 +4069,7 @@
         <v>29</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>58</v>
@@ -2751,10 +4078,10 @@
         <v>59</v>
       </c>
       <c r="I28" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="J28" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>196</v>
       </c>
       <c r="M28" s="17">
         <f t="shared" si="0"/>
@@ -2787,7 +4114,7 @@
         <v>26</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J29" s="9" t="s">
         <v>107</v>
@@ -2958,10 +4285,10 @@
         <v>153</v>
       </c>
       <c r="I33" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>155</v>
       </c>
       <c r="K33" s="9">
         <v>258</v>
@@ -3159,7 +4486,7 @@
         <v>92</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>96</v>
@@ -3168,10 +4495,10 @@
         <v>97</v>
       </c>
       <c r="I38" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="J38" s="9" t="s">
         <v>213</v>
-      </c>
-      <c r="J38" s="9" t="s">
-        <v>214</v>
       </c>
       <c r="K38" s="9">
         <v>96</v>
@@ -3201,19 +4528,19 @@
         <v>29</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H39" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="J39" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>216</v>
       </c>
       <c r="K39" s="9">
         <v>56</v>
@@ -3369,19 +4696,19 @@
         <v>29</v>
       </c>
       <c r="F43" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="H43" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="H43" s="9" t="s">
+      <c r="I43" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="I43" s="9" t="s">
+      <c r="J43" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>180</v>
       </c>
       <c r="K43" s="9">
         <v>486</v>
@@ -3411,19 +4738,19 @@
         <v>92</v>
       </c>
       <c r="F44" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="I44" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="I44" s="9" t="s">
+      <c r="J44" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="J44" s="9" t="s">
-        <v>227</v>
       </c>
       <c r="K44" s="9">
         <v>264</v>
@@ -3453,7 +4780,7 @@
         <v>92</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>25</v>
@@ -3462,10 +4789,10 @@
         <v>26</v>
       </c>
       <c r="I45" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="J45" s="9" t="s">
         <v>220</v>
-      </c>
-      <c r="J45" s="9" t="s">
-        <v>221</v>
       </c>
       <c r="K45" s="9">
         <v>434</v>
@@ -3527,19 +4854,19 @@
         <v>92</v>
       </c>
       <c r="F47" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G47" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I47" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="J47" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="J47" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="K47" s="9">
         <v>245</v>
@@ -3569,19 +4896,19 @@
         <v>92</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>71</v>
       </c>
       <c r="H48" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="I48" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="I48" s="9" t="s">
+      <c r="J48" s="9" t="s">
         <v>192</v>
-      </c>
-      <c r="J48" s="9" t="s">
-        <v>193</v>
       </c>
       <c r="K48" s="9">
         <v>257</v>
@@ -3676,67 +5003,262 @@
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="10"/>
-      <c r="F51" s="23"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="M51" s="18">
+    <row r="51" spans="1:13" s="24" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="35">
+        <v>50</v>
+      </c>
+      <c r="B51" s="33">
+        <v>43083</v>
+      </c>
+      <c r="C51" s="33">
+        <v>43083</v>
+      </c>
+      <c r="D51" s="23">
+        <v>100</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="G51" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="H51" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="I51" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="J51" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="K51" s="23">
+        <v>264</v>
+      </c>
+      <c r="L51" s="23">
+        <v>8</v>
+      </c>
+      <c r="M51" s="36">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
-      <c r="F52" s="23"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
+        <v>138.66666666666666</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="27" x14ac:dyDescent="0.25">
+      <c r="A52" s="16">
+        <v>51</v>
+      </c>
+      <c r="B52" s="20">
+        <v>43083</v>
+      </c>
+      <c r="C52" s="33">
+        <v>43083</v>
+      </c>
+      <c r="D52" s="9">
+        <v>101</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G52" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="H52" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="K52" s="9">
+        <v>553</v>
+      </c>
+      <c r="L52" s="9">
+        <v>8</v>
+      </c>
       <c r="M52" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="10"/>
-      <c r="F53" s="23"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
+        <v>170.77777777777777</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="81" x14ac:dyDescent="0.25">
+      <c r="A53" s="16">
+        <v>52</v>
+      </c>
+      <c r="B53" s="20">
+        <v>43083</v>
+      </c>
+      <c r="C53" s="33">
+        <v>43083</v>
+      </c>
+      <c r="D53" s="9">
+        <v>111</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="G53" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="H53" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="J53" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="K53" s="9">
+        <v>170</v>
+      </c>
+      <c r="L53" s="9">
+        <v>74</v>
+      </c>
       <c r="M53" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="10"/>
-      <c r="F54" s="23"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
+        <v>113.55555555555556</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="16">
+        <v>53</v>
+      </c>
+      <c r="B54" s="20">
+        <v>43083</v>
+      </c>
+      <c r="C54" s="33">
+        <v>43083</v>
+      </c>
+      <c r="D54" s="9">
+        <v>112</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F54" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="G54" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="H54" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="K54" s="9">
+        <v>210</v>
+      </c>
+      <c r="L54" s="9">
+        <v>69</v>
+      </c>
       <c r="M54" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="10"/>
-      <c r="F55" s="23"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
+        <v>119.11111111111111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="54" x14ac:dyDescent="0.25">
+      <c r="A55" s="16">
+        <v>54</v>
+      </c>
+      <c r="B55" s="20">
+        <v>43083</v>
+      </c>
+      <c r="C55" s="33">
+        <v>43083</v>
+      </c>
+      <c r="D55" s="9">
+        <v>113</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="F55" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="G55" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="H55" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="J55" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K55" s="9">
+        <v>197</v>
+      </c>
+      <c r="L55" s="9">
+        <v>7</v>
+      </c>
       <c r="M55" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="10"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
+        <v>131.44444444444446</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="16">
+        <v>55</v>
+      </c>
+      <c r="B56" s="20">
+        <v>43083</v>
+      </c>
+      <c r="C56" s="33">
+        <v>43083</v>
+      </c>
+      <c r="D56" s="9">
+        <v>226</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="G56" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="H56" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="J56" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="K56" s="9">
+        <v>353</v>
+      </c>
+      <c r="L56" s="9">
+        <v>8</v>
+      </c>
       <c r="M56" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>148.55555555555554</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="10"/>
+      <c r="A57" s="16">
+        <v>56</v>
+      </c>
       <c r="F57" s="23"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
@@ -3746,7 +5268,9 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="10"/>
+      <c r="A58" s="16">
+        <v>57</v>
+      </c>
       <c r="F58" s="23"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
@@ -3756,7 +5280,9 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="10"/>
+      <c r="A59" s="16">
+        <v>58</v>
+      </c>
       <c r="F59" s="23"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
@@ -3766,7 +5292,9 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="10"/>
+      <c r="A60" s="16">
+        <v>59</v>
+      </c>
       <c r="F60" s="23"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
@@ -3776,7 +5304,9 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="10"/>
+      <c r="A61" s="16">
+        <v>60</v>
+      </c>
       <c r="F61" s="23"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
@@ -3786,7 +5316,9 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="10"/>
+      <c r="A62" s="16">
+        <v>61</v>
+      </c>
       <c r="F62" s="23"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
@@ -3796,7 +5328,9 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63" s="10"/>
+      <c r="A63" s="16">
+        <v>62</v>
+      </c>
       <c r="F63" s="23"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
@@ -3805,8 +5339,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64" s="10"/>
+    <row r="64" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A64" s="16">
+        <v>63</v>
+      </c>
+      <c r="B64" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="C64" s="29" t="s">
+        <v>254</v>
+      </c>
       <c r="F64" s="23"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
@@ -3815,8 +5357,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A65" s="10"/>
+    <row r="65" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A65" s="16">
+        <v>64</v>
+      </c>
+      <c r="B65" s="30">
+        <v>226</v>
+      </c>
+      <c r="C65" s="31" t="str">
+        <f>IF(COUNTIF(D:D,B65),"Done","Not Yet")</f>
+        <v>Done</v>
+      </c>
       <c r="F65" s="23"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
@@ -3826,7 +5377,9 @@
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="10"/>
+      <c r="A66" s="16">
+        <v>65</v>
+      </c>
       <c r="F66" s="23"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
@@ -3836,7 +5389,9 @@
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A67" s="10"/>
+      <c r="A67" s="16">
+        <v>66</v>
+      </c>
       <c r="F67" s="23"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
@@ -11378,28 +12933,28 @@
       <c r="M1008" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G1007"/>
+  <autoFilter ref="H1:H1008"/>
   <sortState ref="A2:N1008">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="7"/>
   <conditionalFormatting sqref="M1:M1008">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1008">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH(("Easy"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1008">
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH(("Medium"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="C1:C50 C66:C1048576 C58:C59 C62:C64">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>43070</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11410,6 +12965,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D1012"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -17958,42 +19514,42 @@
   </sheetData>
   <phoneticPr fontId="7"/>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Algo">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Algo">
       <formula>NOT(ISERROR(SEARCH(("Algo"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Array">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Array">
       <formula>NOT(ISERROR(SEARCH(("Array"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Backtracking">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Backtracking">
       <formula>NOT(ISERROR(SEARCH(("Backtracking"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="DP">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="DP">
       <formula>NOT(ISERROR(SEARCH(("DP"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="LinkedList">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="LinkedList">
       <formula>NOT(ISERROR(SEARCH(("LinkedList"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Math">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Math">
       <formula>NOT(ISERROR(SEARCH(("Math"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Tree">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="Tree">
       <formula>NOT(ISERROR(SEARCH(("Tree"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="String">
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="String">
       <formula>NOT(ISERROR(SEARCH(("String"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>